<commit_message>
feat: implement automatic lesson progress tracking and fix navigation
</commit_message>
<xml_diff>
--- a/data/excel/مقرر مادة التربية الإسلامية أولى بكالوريا.xlsx
+++ b/data/excel/مقرر مادة التربية الإسلامية أولى بكالوريا.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30b93018d7010778/Documents/Classroom Management System/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabil\Projects\Classroom-Management-System\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{9E85D955-FD15-4DF4-AB58-A4C7FA41E884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F1C7F7C-7A7B-445B-AF2B-1158D0508C47}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E1ADE1-D1F6-48A1-B133-ACCCE2839470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F914882B-0A48-40F1-99DA-01E8B18757DB}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="32">
   <si>
     <t>تقويم تشخيصي</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>أولى بكالوريا</t>
+  </si>
+  <si>
+    <t>الحصص</t>
   </si>
 </sst>
 </file>
@@ -953,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F491B371-0DDE-4C57-A6F3-3D3A75B98413}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -966,7 +969,7 @@
     <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -979,8 +982,11 @@
       <c r="D1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -993,8 +999,11 @@
       <c r="D2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1007,8 +1016,11 @@
       <c r="D3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1021,8 +1033,11 @@
       <c r="D4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1035,8 +1050,11 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1049,8 +1067,11 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1063,8 +1084,11 @@
       <c r="D7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1077,8 +1101,11 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1091,8 +1118,11 @@
       <c r="D9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1105,8 +1135,11 @@
       <c r="D10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1119,8 +1152,11 @@
       <c r="D11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1133,8 +1169,11 @@
       <c r="D12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1147,8 +1186,11 @@
       <c r="D13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1161,8 +1203,11 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1175,8 +1220,11 @@
       <c r="D15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1189,8 +1237,11 @@
       <c r="D16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1203,8 +1254,11 @@
       <c r="D17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1217,8 +1271,11 @@
       <c r="D18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1231,8 +1288,11 @@
       <c r="D19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1245,8 +1305,11 @@
       <c r="D20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1259,8 +1322,11 @@
       <c r="D21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1273,8 +1339,11 @@
       <c r="D22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1287,8 +1356,11 @@
       <c r="D23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1301,8 +1373,11 @@
       <c r="D24" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1315,8 +1390,11 @@
       <c r="D25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1329,8 +1407,11 @@
       <c r="D26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1343,8 +1424,11 @@
       <c r="D27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1357,8 +1441,11 @@
       <c r="D28" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1371,8 +1458,11 @@
       <c r="D29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1385,8 +1475,11 @@
       <c r="D30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1399,8 +1492,11 @@
       <c r="D31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1413,8 +1509,11 @@
       <c r="D32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1427,8 +1526,11 @@
       <c r="D33" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1441,8 +1543,11 @@
       <c r="D34" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1454,6 +1559,9 @@
       </c>
       <c r="D35" t="s">
         <v>30</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>